<commit_message>
Successful class choosing from GA algorithm
</commit_message>
<xml_diff>
--- a/Schedule_Template.xlsx
+++ b/Schedule_Template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin Ngo\Desktop\Projects\Scheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kevin/Desktop/Random Code/Class-Base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{166ACD24-ADEE-4780-918A-C73003573EF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Class Schedule" sheetId="2" r:id="rId1"/>
@@ -19,8 +18,6 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Class Schedule'!$B$3:$I$56</definedName>
     <definedName name="Cal_Endtime">0.999305555555556</definedName>
-    <definedName name="ColumnTitle2">ClassList[[#Headers],[CLASS]]</definedName>
-    <definedName name="ColumnTitleRegion..H2.1">'Class Schedule'!$G$1</definedName>
     <definedName name="CurrentTime">TIME(HOUR(NOW()),MINUTE(NOW()),SECOND(NOW()))</definedName>
     <definedName name="Increment">TIME(0,MinuteInterval,0)</definedName>
     <definedName name="LastRow">MAX(MATCH(9.99E+307,'Class Schedule'!$B:$B),MATCH(REPT("z",255),'Class Schedule'!$B:$B))</definedName>
@@ -33,23 +30,50 @@
     <definedName name="ThisRow">'Class Schedule'!$C1:$I1</definedName>
     <definedName name="ThisWeekday">CHOOSE(WEEKDAY(TODAY()),"Sunday","Monday","Tuesday","Wednesday","Thursday","Friday","Saturday")</definedName>
     <definedName name="Times">ClassSchedule[TIME]</definedName>
-    <definedName name="Title1">ClassSchedule[[#Headers],[TIME]]</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
+  <si>
+    <t>Technical Writing</t>
+  </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>WR-121</t>
+  </si>
+  <si>
+    <t>Public Speaking</t>
+  </si>
+  <si>
+    <t>SP-111</t>
+  </si>
+  <si>
+    <t>Algebra</t>
+  </si>
+  <si>
+    <t>MTH-113</t>
+  </si>
+  <si>
+    <t>Building A</t>
+  </si>
+  <si>
+    <t>Building B</t>
+  </si>
+  <si>
+    <t>Building C</t>
   </si>
   <si>
     <t>CLASS SCHEDULE</t>
@@ -109,16 +133,28 @@
     <t>15 MIN</t>
   </si>
   <si>
+    <t>Health &amp; Fitness</t>
+  </si>
+  <si>
+    <t>HPE-295</t>
+  </si>
+  <si>
     <t>Class List</t>
   </si>
   <si>
     <t>Class Schedule</t>
   </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>World</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode=";;;@"/>
@@ -260,7 +296,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -293,6 +329,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="6" applyFill="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="5" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -311,8 +356,8 @@
     <cellStyle name="Heading 4" xfId="2" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Table_Details" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Time" xfId="5" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Table_Details" xfId="6"/>
+    <cellStyle name="Time" xfId="5"/>
   </cellStyles>
   <dxfs count="26">
     <dxf>
@@ -625,14 +670,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Class Schedule" defaultPivotStyle="PivotStyleMedium15">
-    <tableStyle name="Class Schedule" pivot="0" count="5" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Class Schedule" pivot="0" count="5">
       <tableStyleElement type="wholeTable" dxfId="25"/>
       <tableStyleElement type="headerRow" dxfId="24"/>
       <tableStyleElement type="totalRow" dxfId="23"/>
       <tableStyleElement type="lastColumn" dxfId="22"/>
       <tableStyleElement type="firstRowStripe" dxfId="21"/>
     </tableStyle>
-    <tableStyle name="Class Schedule Slicer" pivot="0" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="Class Schedule Slicer" pivot="0" table="0" count="10">
       <tableStyleElement type="wholeTable" dxfId="20"/>
       <tableStyleElement type="headerRow" dxfId="19"/>
     </tableStyle>
@@ -918,7 +963,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Select to navigate to Class List worksheet"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C3B1660-A286-46BC-8C75-5618DCAA2DCA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C3B1660-A286-46BC-8C75-5618DCAA2DCA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1002,7 +1047,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Select to navigate to Class Schedule worksheet"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3827567C-2444-4A9B-8BA7-9AD7F5973BFF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3827567C-2444-4A9B-8BA7-9AD7F5973BFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1066,35 +1111,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ClassSchedule" displayName="ClassSchedule" ref="B3:I56" headerRowCellStyle="Heading 4">
-  <autoFilter ref="B3:I56" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="ClassSchedule" displayName="ClassSchedule" ref="B3:I56" headerRowCellStyle="Heading 4">
+  <autoFilter ref="B3:I56"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TIME" totalsRowLabel="Total" dataCellStyle="Time">
+    <tableColumn id="1" name="TIME" totalsRowLabel="Total" dataCellStyle="Time">
       <calculatedColumnFormula>B3+Increment</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SUNDAY" dataDxfId="6" dataCellStyle="Table_Details">
+    <tableColumn id="2" name="SUNDAY" dataDxfId="6" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MONDAY" dataDxfId="5" dataCellStyle="Table_Details">
+    <tableColumn id="3" name="MONDAY" dataDxfId="5" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="TUESDAY" dataDxfId="4" dataCellStyle="Table_Details">
+    <tableColumn id="4" name="TUESDAY" dataDxfId="4" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="WEDNESDAY" dataDxfId="3" dataCellStyle="Table_Details">
+    <tableColumn id="5" name="WEDNESDAY" dataDxfId="3" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="THURSDAY" dataDxfId="2" dataCellStyle="Table_Details">
+    <tableColumn id="6" name="THURSDAY" dataDxfId="2" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FRIDAY" dataDxfId="1" dataCellStyle="Table_Details">
+    <tableColumn id="7" name="FRIDAY" dataDxfId="1" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="SATURDAY" totalsRowFunction="sum" dataCellStyle="Table_Details">
+    <tableColumn id="8" name="SATURDAY" totalsRowFunction="sum" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+  <tableStyleInfo name="Class Schedule" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
       <x14:table altTextSummary="List of classes arranged by weekday &amp; time interval. Class ID is displayed at the intersection of Weekday &amp; Start Time and extends through End Time"/>
@@ -1104,20 +1149,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="ClassList" displayName="ClassList" ref="B2:H10" totalsRowShown="0">
-  <autoFilter ref="B2:H10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ClassList" displayName="ClassList" ref="B2:H25" totalsRowShown="0">
+  <autoFilter ref="B2:H25"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CLASS" dataCellStyle="Table_Details"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ID" dataCellStyle="Table_Details"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="DAY" dataCellStyle="Table_Details"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="LOCATION" dataCellStyle="Table_Details"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="START TIME" dataCellStyle="Time"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="END TIME" dataCellStyle="Time"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="UNIQUE" dataDxfId="0">
+    <tableColumn id="1" name="CLASS" dataCellStyle="Table_Details"/>
+    <tableColumn id="2" name="ID" dataCellStyle="Table_Details"/>
+    <tableColumn id="3" name="DAY" dataCellStyle="Table_Details"/>
+    <tableColumn id="5" name="LOCATION" dataCellStyle="Table_Details"/>
+    <tableColumn id="4" name="START TIME" dataCellStyle="Time"/>
+    <tableColumn id="6" name="END TIME" dataCellStyle="Time"/>
+    <tableColumn id="7" name="UNIQUE" dataDxfId="0">
       <calculatedColumnFormula>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="Class Schedule" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
       <x14:table altTextSummary="Information for classes that display on Class Schedule sheet such as Class, ID, Day (weekday), Location, Start Time &amp; End Time"/>
@@ -1352,86 +1397,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.79998168889431442"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+    <sheetView showGridLines="0" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="1" customWidth="1"/>
     <col min="3" max="8" width="18.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.75" style="1" customWidth="1"/>
-    <col min="10" max="10" width="2.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+    <row r="1" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
       <c r="G2" s="7">
         <v>0.33333333333333331</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="12"/>
-    </row>
-    <row r="3" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>10</v>
-      </c>
       <c r="I3" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="5">
         <f>ScheduleStart</f>
         <v>0.33333333333333331</v>
@@ -1465,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="5">
         <f t="shared" ref="B5:B36" si="0">B4+Increment</f>
         <v>0.34375</v>
@@ -1474,32 +1519,32 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="E5" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="G5" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="I5" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="5">
         <f t="shared" si="0"/>
         <v>0.35416666666666669</v>
@@ -1508,32 +1553,32 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B6&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B6&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="E6" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B6&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B6&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="G6" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B6&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B6&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="I6" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B6&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="5">
         <f t="shared" si="0"/>
         <v>0.36458333333333337</v>
@@ -1542,32 +1587,32 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B7&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B7&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="E7" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B7&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B7&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="G7" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B7&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B7&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="I7" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B7&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="5">
         <f t="shared" si="0"/>
         <v>0.37500000000000006</v>
@@ -1576,32 +1621,32 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B8&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B8&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="E8" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B8&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B8&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="G8" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B8&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B8&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="I8" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B8&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="5">
         <f t="shared" si="0"/>
         <v>0.38541666666666674</v>
@@ -1610,32 +1655,32 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B9&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B9&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="E9" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B9&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B9&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="G9" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B9&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B9&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>MTH-113</v>
       </c>
       <c r="I9" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B9&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="5">
         <f t="shared" si="0"/>
         <v>0.39583333333333343</v>
@@ -1669,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5">
         <f t="shared" si="0"/>
         <v>0.40625000000000011</v>
@@ -1703,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5">
         <f t="shared" si="0"/>
         <v>0.4166666666666668</v>
@@ -1737,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5">
         <f t="shared" si="0"/>
         <v>0.42708333333333348</v>
@@ -1771,7 +1816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="5">
         <f t="shared" si="0"/>
         <v>0.43750000000000017</v>
@@ -1805,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5">
         <f t="shared" si="0"/>
         <v>0.44791666666666685</v>
@@ -1839,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="5">
         <f t="shared" si="0"/>
         <v>0.45833333333333354</v>
@@ -1852,17 +1897,17 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B16&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B16&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>HPE-295</v>
       </c>
       <c r="F16" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B16&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B16&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>HPE-295</v>
       </c>
       <c r="H16" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B16&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -1873,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="5">
         <f t="shared" si="0"/>
         <v>0.46875000000000022</v>
@@ -1886,17 +1931,17 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B17&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B17&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>HPE-295</v>
       </c>
       <c r="F17" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B17&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B17&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>HPE-295</v>
       </c>
       <c r="H17" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B17&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -1907,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="5">
         <f t="shared" si="0"/>
         <v>0.47916666666666691</v>
@@ -1920,17 +1965,17 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B18,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B18&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B18,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B18&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>HPE-295</v>
       </c>
       <c r="F18" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B18,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B18&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B18,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B18&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>HPE-295</v>
       </c>
       <c r="H18" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B18,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B18&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -1941,7 +1986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="5">
         <f t="shared" si="0"/>
         <v>0.48958333333333359</v>
@@ -1954,17 +1999,17 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B19,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B19&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B19,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B19&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>HPE-295</v>
       </c>
       <c r="F19" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B19,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B19&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B19,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B19&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>HPE-295</v>
       </c>
       <c r="H19" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B19,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B19&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -1975,7 +2020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="5">
         <f t="shared" si="0"/>
         <v>0.50000000000000022</v>
@@ -1988,17 +2033,17 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B20,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B20&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B20,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B20&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>HPE-295</v>
       </c>
       <c r="F20" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B20,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B20&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B20,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B20&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>HPE-295</v>
       </c>
       <c r="H20" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B20,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B20&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -2009,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="5">
         <f t="shared" si="0"/>
         <v>0.51041666666666685</v>
@@ -2043,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="5">
         <f t="shared" si="0"/>
         <v>0.52083333333333348</v>
@@ -2077,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23"/>
       <c r="B23" s="5">
         <f t="shared" si="0"/>
@@ -2112,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24"/>
       <c r="B24" s="5">
         <f t="shared" si="0"/>
@@ -2122,17 +2167,17 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B24,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B24&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B24,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B24&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>WR-121</v>
       </c>
       <c r="E24" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B24,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B24&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B24,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B24&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>WR-121</v>
       </c>
       <c r="G24" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B24,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B24&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -2147,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="5">
         <f t="shared" si="0"/>
         <v>0.55208333333333337</v>
@@ -2156,17 +2201,17 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B25,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B25&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B25,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B25&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>WR-121</v>
       </c>
       <c r="E25" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B25,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B25&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B25,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B25&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>WR-121</v>
       </c>
       <c r="G25" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B25,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B25&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -2181,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="5">
         <f t="shared" si="0"/>
         <v>0.5625</v>
@@ -2190,17 +2235,17 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B26,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B26&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B26,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B26&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>WR-121</v>
       </c>
       <c r="E26" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B26,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B26&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B26,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B26&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>WR-121</v>
       </c>
       <c r="G26" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B26,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B26&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -2215,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="5">
         <f t="shared" si="0"/>
         <v>0.57291666666666663</v>
@@ -2224,17 +2269,17 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B27,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B27&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B27,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B27&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>WR-121</v>
       </c>
       <c r="E27" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B27,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B27&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B27,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B27&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>WR-121</v>
       </c>
       <c r="G27" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B27,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B27&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -2249,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="5">
         <f t="shared" si="0"/>
         <v>0.58333333333333326</v>
@@ -2258,17 +2303,17 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B28,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B28&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B28,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B28&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>WR-121</v>
       </c>
       <c r="E28" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B28,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B28&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B28,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B28&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>WR-121</v>
       </c>
       <c r="G28" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B28,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B28&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -2283,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="5">
         <f t="shared" si="0"/>
         <v>0.59374999999999989</v>
@@ -2317,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="5">
         <f t="shared" si="0"/>
         <v>0.60416666666666652</v>
@@ -2351,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="5">
         <f t="shared" si="0"/>
         <v>0.61458333333333315</v>
@@ -2385,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="5">
         <f t="shared" si="0"/>
         <v>0.62499999999999978</v>
@@ -2419,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="5">
         <f t="shared" si="0"/>
         <v>0.63541666666666641</v>
@@ -2453,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="5">
         <f t="shared" si="0"/>
         <v>0.64583333333333304</v>
@@ -2487,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="5">
         <f t="shared" si="0"/>
         <v>0.65624999999999967</v>
@@ -2521,7 +2566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="5">
         <f t="shared" si="0"/>
         <v>0.6666666666666663</v>
@@ -2530,9 +2575,9 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B36,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B36&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D36" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B36,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B36&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>SP-111</v>
       </c>
       <c r="E36" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B36,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B36&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -2555,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="5">
         <f t="shared" ref="B37:B56" si="1">B36+Increment</f>
         <v>0.67708333333333293</v>
@@ -2564,9 +2609,9 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B37,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B37&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B37,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B37&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>SP-111</v>
       </c>
       <c r="E37" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B37,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B37&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -2589,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="5">
         <f t="shared" si="1"/>
         <v>0.68749999999999956</v>
@@ -2598,9 +2643,9 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B38,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B38&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D38" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B38,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B38&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>SP-111</v>
       </c>
       <c r="E38" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B38,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B38&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -2623,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="5">
         <f t="shared" si="1"/>
         <v>0.69791666666666619</v>
@@ -2632,9 +2677,9 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B39,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B39&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D39" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B39,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B39&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>SP-111</v>
       </c>
       <c r="E39" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B39,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B39&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -2657,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="5">
         <f t="shared" si="1"/>
         <v>0.70833333333333282</v>
@@ -2666,9 +2711,9 @@
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B40,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B40&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D40" s="8" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B40,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B40&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
-        <v>0</v>
+        <v>SP-111</v>
       </c>
       <c r="E40" s="8">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B40,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B40&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
@@ -2691,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="5">
         <f t="shared" si="1"/>
         <v>0.71874999999999944</v>
@@ -2725,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="5">
         <f t="shared" si="1"/>
         <v>0.72916666666666607</v>
@@ -2759,7 +2804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="5">
         <f t="shared" si="1"/>
         <v>0.7395833333333327</v>
@@ -2793,7 +2838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="5">
         <f t="shared" si="1"/>
         <v>0.74999999999999933</v>
@@ -2827,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="5">
         <f t="shared" si="1"/>
         <v>0.76041666666666596</v>
@@ -2861,7 +2906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="5">
         <f t="shared" si="1"/>
         <v>0.77083333333333259</v>
@@ -2895,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="5">
         <f t="shared" si="1"/>
         <v>0.78124999999999922</v>
@@ -2929,7 +2974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="5">
         <f t="shared" si="1"/>
         <v>0.79166666666666585</v>
@@ -2963,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B49" s="5">
         <f t="shared" si="1"/>
         <v>0.80208333333333248</v>
@@ -2997,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="5">
         <f t="shared" si="1"/>
         <v>0.81249999999999911</v>
@@ -3031,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="5">
         <f t="shared" si="1"/>
         <v>0.82291666666666574</v>
@@ -3065,7 +3110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="5">
         <f t="shared" si="1"/>
         <v>0.83333333333333237</v>
@@ -3099,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="5">
         <f t="shared" si="1"/>
         <v>0.843749999999999</v>
@@ -3133,7 +3178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="5">
         <f t="shared" si="1"/>
         <v>0.85416666666666563</v>
@@ -3167,7 +3212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B55" s="5">
         <f t="shared" si="1"/>
         <v>0.86458333333333226</v>
@@ -3201,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B56" s="5">
         <f t="shared" si="1"/>
         <v>0.87499999999999889</v>
@@ -3284,29 +3329,29 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a start time from the list. Select CANCEL, and then press ALT+DOWN ARROW to select start time from the drop-down list" prompt="Enter schedule start time in this cell. Press ALT+DOWN ARROW to open the drop-down list, and then press ENTER to select the time" sqref="G2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a start time from the list. Select CANCEL, and then press ALT+DOWN ARROW to select start time from the drop-down list" prompt="Enter schedule start time in this cell. Press ALT+DOWN ARROW to open the drop-down list, and then press ENTER to select the time" sqref="G2">
       <formula1>"8:00 AM,9:00 AM,10:00 AM,11:00 AM,12:00 PM,1:00 PM,2:00 PM,3:00 PM,4:00 PM,5:00 PM"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a time interval from the list. Select CANCEL, and then press ALT+DOWN ARROW to select time interval from the drop-down list" prompt="Enter time interval in this cell. Press ALT+DOWN ARROW to open the drop-down list, and then press ENTER to select time interval" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a time interval from the list. Select CANCEL, and then press ALT+DOWN ARROW to select time interval from the drop-down list" prompt="Enter time interval in this cell. Press ALT+DOWN ARROW to open the drop-down list, and then press ENTER to select time interval" sqref="H2">
       <formula1>"15 MIN,20 MIN,30 MIN,40 MIN,45 MIN,60 MIN"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="To update Class Schedule, modify Schedule Start in cell G2 &amp; Time Interval in cell H2. Add class information in Class List worksheet. Cell I1 navigates to Class List worksheet" sqref="A1" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class Schedule Table, below, is automatically updated from entries in the Class List table in the Class List worksheet. Add rows to the end of the table to extend the schedule" sqref="B1:F2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter schedule start time in cell G2" sqref="G1" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter time interval in cell H2" sqref="H1" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Sunday is automatically updated using entries from Class List worksheet" sqref="C3" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Monday is automatically updated using entries from Class List worksheet" sqref="D3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Tuesday is automatically updated using entries from Class List worksheet" sqref="E3" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Wednesday is automatically updated using entries from Class List worksheet" sqref="F3" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Thursday is automatically updated using entries from Class List worksheet" sqref="G3" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Friday is automatically updated using entries from Class List worksheet" sqref="H3" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Saturday is automatically updated using entries from Class List worksheet" sqref="I3" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This column is generated based on Start Time in cell G2 and Time Interval in cell H2" sqref="B3" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigational link to Class List worksheet" sqref="I1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Schedule start time determined by the time entered in cell G2" sqref="B4" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="To update Class Schedule, modify Schedule Start in cell G2 &amp; Time Interval in cell H2. Add class information in Class List worksheet. Cell I1 navigates to Class List worksheet" sqref="A1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class Schedule Table, below, is automatically updated from entries in the Class List table in the Class List worksheet. Add rows to the end of the table to extend the schedule" sqref="B1:F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter schedule start time in cell G2" sqref="G1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter time interval in cell H2" sqref="H1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Sunday is automatically updated using entries from Class List worksheet" sqref="C3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Monday is automatically updated using entries from Class List worksheet" sqref="D3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Tuesday is automatically updated using entries from Class List worksheet" sqref="E3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Wednesday is automatically updated using entries from Class List worksheet" sqref="F3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Thursday is automatically updated using entries from Class List worksheet" sqref="G3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Friday is automatically updated using entries from Class List worksheet" sqref="H3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Saturday is automatically updated using entries from Class List worksheet" sqref="I3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This column is generated based on Start Time in cell G2 and Time Interval in cell H2" sqref="B3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Schedule start time determined by the time entered in cell G2" sqref="B4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to Class List worksheet" sqref="I1:I2"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I1" location="'Class List'!A1" tooltip="Select to navigate to Class List worksheet" display="Class List" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I1" location="'Class List'!A1" tooltip="Select to navigate to Class List worksheet" display="Class List"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3325,159 +3370,463 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet2">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0">
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H10"/>
+  <dimension ref="B1:H25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="1" customWidth="1"/>
-    <col min="5" max="7" width="22.25" style="1" customWidth="1"/>
+    <col min="5" max="7" width="22.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.5" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="2.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="2.6640625" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="13" t="s">
+    <row r="1" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="E3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.54166666666666596</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="H3" s="2">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+    <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.54166666666666596</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="H4" s="2">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="H5" s="2">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.5</v>
+      </c>
       <c r="H6" s="2">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.45833333333333287</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.5</v>
+      </c>
       <c r="H7" s="2">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.38541666666666669</v>
+      </c>
       <c r="H8" s="2">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.38541666666666669</v>
+      </c>
       <c r="H9" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.38541666666666669</v>
+      </c>
       <c r="H10" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="3">
+        <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3486,21 +3835,21 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <dataValidations count="10">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigational link to Class Schedule worksheet" sqref="G1:H1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Class in this column" sqref="B2" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class ID in this column" sqref="C2" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class Day in this column.  In each cell of this column, Press ALT+DOWN ARROW to open the drop-down list, and then press ENTER to select the Day" sqref="D2" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class Location in this column" sqref="E2" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class Start Time in this column" sqref="F2" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class End Time in this column" sqref="G2" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a class list to update Class Schedule by updating the Class List table. Use table filters to get specific class or date. Cell G1 navigates to Class Schedule" sqref="A1" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This list is used to create the Class Schedule on the Class Schedule worksheet. Update the Class List table, below, to automatically update Class Schedule" sqref="B1:F1" xr:uid="{00000000-0002-0000-0100-000008000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a day from the list. Select CANCEL, and then press ALT+DOWN ARROW to select from the drop-down list" sqref="D3:D10" xr:uid="{00000000-0002-0000-0100-000009000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to Class Schedule worksheet" sqref="G1:H1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Class in this column" sqref="B2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class ID in this column" sqref="C2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class Day in this column.  In each cell of this column, Press ALT+DOWN ARROW to open the drop-down list, and then press ENTER to select the Day" sqref="D2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class Location in this column" sqref="E2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class Start Time in this column" sqref="F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class End Time in this column" sqref="G2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a class list to update Class Schedule by updating the Class List table. Use table filters to get specific class or date. Cell G1 navigates to Class Schedule" sqref="A1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This list is used to create the Class Schedule on the Class Schedule worksheet. Update the Class List table, below, to automatically update Class Schedule" sqref="B1:F1"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a day from the list. Select CANCEL, and then press ALT+DOWN ARROW to select from the drop-down list" sqref="D3:D25">
       <formula1>"SUNDAY,MONDAY,TUESDAY,WEDNESDAY,THURSDAY,FRIDAY,SATURDAY"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G1:H1" location="'Class Schedule'!A1" tooltip="Select to navigate to Class Schedule worksheet" display="Class Schedule" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G1:H1" location="'Class Schedule'!A1" tooltip="Select to navigate to Class Schedule worksheet" display="Class Schedule"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fully working - commented script
</commit_message>
<xml_diff>
--- a/Schedule_Template.xlsx
+++ b/Schedule_Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kevin/Desktop/Random Code/Class-Base/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin Ngo\Desktop\Class-Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BE38C5-6E03-4794-A844-4171DCF60C3B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="20535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Class Schedule" sheetId="2" r:id="rId1"/>
@@ -31,18 +32,18 @@
     <definedName name="ThisWeekday">CHOOSE(WEEKDAY(TODAY()),"Sunday","Monday","Tuesday","Wednesday","Thursday","Friday","Saturday")</definedName>
     <definedName name="Times">ClassSchedule[TIME]</definedName>
   </definedNames>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -159,7 +160,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode=";;;@"/>
@@ -301,7 +302,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -313,44 +314,50 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="5">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="3">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="18" fontId="2" fillId="2" borderId="2" xfId="4" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="6">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="6" applyFill="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="5" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="7" applyBorder="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="7">
       <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -361,30 +368,69 @@
     <cellStyle name="Heading 4" xfId="2" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Table_Details" xfId="6"/>
-    <cellStyle name="Time" xfId="5"/>
+    <cellStyle name="Table_Details" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Time" xfId="5" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="37">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -675,16 +721,16 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Class Schedule" defaultPivotStyle="PivotStyleMedium15">
-    <tableStyle name="Class Schedule" pivot="0" count="5">
-      <tableStyleElement type="wholeTable" dxfId="25"/>
-      <tableStyleElement type="headerRow" dxfId="24"/>
-      <tableStyleElement type="totalRow" dxfId="23"/>
-      <tableStyleElement type="lastColumn" dxfId="22"/>
-      <tableStyleElement type="firstRowStripe" dxfId="21"/>
+    <tableStyle name="Class Schedule" pivot="0" count="5" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="36"/>
+      <tableStyleElement type="headerRow" dxfId="35"/>
+      <tableStyleElement type="totalRow" dxfId="34"/>
+      <tableStyleElement type="lastColumn" dxfId="33"/>
+      <tableStyleElement type="firstRowStripe" dxfId="32"/>
     </tableStyle>
-    <tableStyle name="Class Schedule Slicer" pivot="0" table="0" count="10">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
-      <tableStyleElement type="headerRow" dxfId="19"/>
+    <tableStyle name="Class Schedule Slicer" pivot="0" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+      <tableStyleElement type="wholeTable" dxfId="31"/>
+      <tableStyleElement type="headerRow" dxfId="30"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -968,7 +1014,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Select to navigate to Class List worksheet"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9C3B1660-A286-46BC-8C75-5618DCAA2DCA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C3B1660-A286-46BC-8C75-5618DCAA2DCA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1052,7 +1098,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Select to navigate to Class Schedule worksheet"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3827567C-2444-4A9B-8BA7-9AD7F5973BFF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3827567C-2444-4A9B-8BA7-9AD7F5973BFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1116,31 +1162,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="ClassSchedule" displayName="ClassSchedule" ref="B3:I56" headerRowCellStyle="Heading 4">
-  <autoFilter ref="B3:I56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ClassSchedule" displayName="ClassSchedule" ref="B3:I56" headerRowDxfId="17" dataDxfId="16" totalsRowDxfId="15" headerRowCellStyle="Heading 4">
+  <autoFilter ref="B3:I56" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="TIME" totalsRowLabel="Total" dataCellStyle="Time">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TIME" totalsRowLabel="Total" dataDxfId="14" dataCellStyle="Time">
       <calculatedColumnFormula>B3+Increment</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="SUNDAY" dataDxfId="6" dataCellStyle="Table_Details">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SUNDAY" dataDxfId="13" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="MONDAY" dataDxfId="5" dataCellStyle="Table_Details">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MONDAY" dataDxfId="12" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="TUESDAY" dataDxfId="4" dataCellStyle="Table_Details">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="TUESDAY" dataDxfId="11" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="WEDNESDAY" dataDxfId="3" dataCellStyle="Table_Details">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="WEDNESDAY" dataDxfId="10" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="THURSDAY" dataDxfId="2" dataCellStyle="Table_Details">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="THURSDAY" dataDxfId="9" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="FRIDAY" dataDxfId="1" dataCellStyle="Table_Details">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FRIDAY" dataDxfId="8" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="SATURDAY" totalsRowFunction="sum" dataCellStyle="Table_Details">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="SATURDAY" totalsRowFunction="sum" dataDxfId="7" dataCellStyle="Table_Details">
       <calculatedColumnFormula>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1154,16 +1200,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ClassList" displayName="ClassList" ref="B2:H25" totalsRowShown="0">
-  <autoFilter ref="B2:H25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="ClassList" displayName="ClassList" ref="B2:H25" totalsRowShown="0">
+  <autoFilter ref="B2:H25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="CLASS" dataCellStyle="Table_Details"/>
-    <tableColumn id="2" name="ID" dataCellStyle="Table_Details"/>
-    <tableColumn id="3" name="DAY" dataCellStyle="Table_Details"/>
-    <tableColumn id="5" name="LOCATION" dataCellStyle="Table_Details"/>
-    <tableColumn id="4" name="START TIME" dataCellStyle="Time"/>
-    <tableColumn id="6" name="END TIME" dataCellStyle="Time"/>
-    <tableColumn id="7" name="UNIQUE" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CLASS" dataDxfId="6" dataCellStyle="Table_Details"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ID" dataDxfId="5" dataCellStyle="Table_Details"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="DAY" dataDxfId="4" dataCellStyle="Table_Details"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="LOCATION" dataDxfId="3" dataCellStyle="Table_Details"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="START TIME" dataDxfId="2" dataCellStyle="Time"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="END TIME" dataDxfId="1" dataCellStyle="Time"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="UNIQUE" dataDxfId="0">
       <calculatedColumnFormula>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1402,1885 +1448,1885 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1">
     <tabColor theme="5" tint="0.79998168889431442"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="1" customWidth="1"/>
-    <col min="3" max="8" width="18.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="2.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" style="10" customWidth="1"/>
+    <col min="3" max="8" width="18.5" style="10" customWidth="1"/>
+    <col min="9" max="9" width="18.625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="2.625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="6" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="7">
+    <row r="2" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="15"/>
-    </row>
-    <row r="3" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="10" t="s">
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="5">
+    <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="8">
         <f>ScheduleStart</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B4,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B4&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="5">
+    <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="8">
         <f t="shared" ref="B5:B36" si="0">B4+Increment</f>
         <v>0.34375</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D5" s="8" t="str">
+      <c r="D5" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F5" s="8" t="str">
+      <c r="F5" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="8" t="str">
+      <c r="H5" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B5,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B5&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="5">
+    <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="8">
         <f t="shared" si="0"/>
         <v>0.35416666666666669</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B6&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="8" t="str">
+      <c r="D6" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B6&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B6&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="8" t="str">
+      <c r="F6" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B6&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B6&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H6" s="8" t="str">
+      <c r="H6" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B6&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B6&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="5">
+    <row r="7" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="8">
         <f t="shared" si="0"/>
         <v>0.36458333333333337</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B7&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="8" t="str">
+      <c r="D7" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B7&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B7&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="8" t="str">
+      <c r="F7" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B7&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B7&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H7" s="8" t="str">
+      <c r="H7" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B7&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B7&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="5">
+    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B8" s="8">
         <f t="shared" si="0"/>
         <v>0.37500000000000006</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B8&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="8" t="str">
+      <c r="D8" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B8&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B8&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="8" t="str">
+      <c r="F8" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B8&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B8&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="8" t="str">
+      <c r="H8" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B8&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B8&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="5">
+    <row r="9" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8">
         <f t="shared" si="0"/>
         <v>0.38541666666666674</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B9&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D9" s="8" t="str">
+      <c r="D9" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B9&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B9&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="8" t="str">
+      <c r="F9" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B9&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B9&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="8" t="str">
+      <c r="H9" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B9&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>MTH-113</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B9&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="5">
+    <row r="10" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="8">
         <f t="shared" si="0"/>
         <v>0.39583333333333343</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B10,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B10&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B10,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B10&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B10,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B10&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B10,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B10&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B10,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B10&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B10,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B10&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B10,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B10&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="5">
+    <row r="11" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8">
         <f t="shared" si="0"/>
         <v>0.40625000000000011</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B11,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B11&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B11,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B11&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B11,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B11&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B11,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B11&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B11,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B11&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B11,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B11&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B11,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B11&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="5">
+    <row r="12" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="8">
         <f t="shared" si="0"/>
         <v>0.4166666666666668</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B12,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B12&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B12,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B12&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B12,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B12&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B12,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B12&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B12,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B12&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B12,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B12&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B12,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B12&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="5">
+    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="8">
         <f t="shared" si="0"/>
         <v>0.42708333333333348</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B13,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B13&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B13,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B13&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B13,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B13&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B13,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B13&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B13,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B13&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B13,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B13&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B13,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B13&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="5">
+    <row r="14" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="8">
         <f t="shared" si="0"/>
         <v>0.43750000000000017</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B14,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B14&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B14,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B14&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B14,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B14&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B14,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B14&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B14,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B14&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B14,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B14&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B14,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B14&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="5">
+    <row r="15" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="8">
         <f t="shared" si="0"/>
         <v>0.44791666666666685</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B15,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B15&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B15,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B15&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B15,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B15&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B15,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B15&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B15,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B15&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B15,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B15&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B15,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B15&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="5">
+    <row r="16" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="8">
         <f t="shared" si="0"/>
         <v>0.45833333333333354</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B16&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B16&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="8" t="str">
+      <c r="E16" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B16&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>HPE-295</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B16&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="8" t="str">
+      <c r="G16" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B16&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>HPE-295</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B16&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B16&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="5">
+    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="8">
         <f t="shared" si="0"/>
         <v>0.46875000000000022</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B17&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B17&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="8" t="str">
+      <c r="E17" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B17&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>HPE-295</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B17&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="8" t="str">
+      <c r="G17" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B17&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>HPE-295</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B17&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B17&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="5">
+    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="8">
         <f t="shared" si="0"/>
         <v>0.47916666666666691</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B18,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B18&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B18,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B18&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="8" t="str">
+      <c r="E18" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B18,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B18&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>HPE-295</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B18,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B18&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="8" t="str">
+      <c r="G18" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B18,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B18&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>HPE-295</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B18,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B18&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B18,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B18&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="5">
+    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="8">
         <f t="shared" si="0"/>
         <v>0.48958333333333359</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B19,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B19&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B19,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B19&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="8" t="str">
+      <c r="E19" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B19,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B19&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>HPE-295</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B19,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B19&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="8" t="str">
+      <c r="G19" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B19,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B19&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>HPE-295</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B19,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B19&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B19,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B19&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="5">
+    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="8">
         <f t="shared" si="0"/>
         <v>0.50000000000000022</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B20,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B20&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B20,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B20&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="8" t="str">
+      <c r="E20" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B20,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B20&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>HPE-295</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B20,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B20&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="8" t="str">
+      <c r="G20" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B20,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B20&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>HPE-295</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B20,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B20&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B20,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B20&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="5">
+    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="8">
         <f t="shared" si="0"/>
         <v>0.51041666666666685</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B21,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B21&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B21,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B21&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B21,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B21&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B21,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B21&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B21,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B21&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B21,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B21&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B21,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B21&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="5">
+    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="8">
         <f t="shared" si="0"/>
         <v>0.52083333333333348</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B22,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B22&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B22,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B22&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B22,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B22&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B22,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B22&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B22,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B22&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B22,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B22&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I22" s="8">
+      <c r="I22" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B22,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B22&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23"/>
-      <c r="B23" s="5">
+      <c r="B23" s="8">
         <f t="shared" si="0"/>
         <v>0.53125000000000011</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B23,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B23&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B23,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B23&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B23,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B23&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B23,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B23&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B23,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B23&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B23,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B23&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I23" s="8">
+      <c r="I23" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B23,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B23&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24"/>
-      <c r="B24" s="5">
+      <c r="B24" s="8">
         <f t="shared" si="0"/>
         <v>0.54166666666666674</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B24,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B24&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="8" t="str">
+      <c r="D24" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B24,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B24&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>WR-121</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B24,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B24&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="8" t="str">
+      <c r="F24" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B24,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B24&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>WR-121</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B24,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B24&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H24" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B24,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B24&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I24" s="8">
+      <c r="I24" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B24,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B24&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="5">
+    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="8">
         <f t="shared" si="0"/>
         <v>0.55208333333333337</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B25,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B25&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="8" t="str">
+      <c r="D25" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B25,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B25&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>WR-121</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B25,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B25&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="8" t="str">
+      <c r="F25" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B25,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B25&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>WR-121</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B25,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B25&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H25" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B25,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B25&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I25" s="8">
+      <c r="I25" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B25,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B25&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="5">
+    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="8">
         <f t="shared" si="0"/>
         <v>0.5625</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B26,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B26&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D26" s="8" t="str">
+      <c r="D26" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B26,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B26&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>WR-121</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B26,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B26&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F26" s="8" t="str">
+      <c r="F26" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B26,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B26&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>WR-121</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B26,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B26&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B26,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B26&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="8">
+      <c r="I26" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B26,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B26&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="5">
+    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="8">
         <f t="shared" si="0"/>
         <v>0.57291666666666663</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B27,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B27&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="8" t="str">
+      <c r="D27" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B27,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B27&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>WR-121</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B27,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B27&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F27" s="8" t="str">
+      <c r="F27" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B27,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B27&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>WR-121</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B27,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B27&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B27,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B27&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I27" s="8">
+      <c r="I27" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B27,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B27&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="5">
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="8">
         <f t="shared" si="0"/>
         <v>0.58333333333333326</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B28,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B28&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D28" s="8" t="str">
+      <c r="D28" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B28,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B28&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>WR-121</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B28,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B28&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="8" t="str">
+      <c r="F28" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B28,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B28&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>WR-121</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B28,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B28&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="8">
+      <c r="H28" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B28,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B28&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I28" s="8">
+      <c r="I28" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B28,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B28&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="5">
+    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="8">
         <f t="shared" si="0"/>
         <v>0.59374999999999989</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B29,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B29&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B29,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B29&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B29,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B29&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B29,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B29&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B29,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B29&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B29,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B29&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="8">
+      <c r="I29" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B29,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B29&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="5">
+    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="8">
         <f t="shared" si="0"/>
         <v>0.60416666666666652</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B30,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B30&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B30,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B30&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B30,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B30&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B30,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B30&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B30,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B30&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B30,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B30&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I30" s="8">
+      <c r="I30" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B30,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B30&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="5">
+    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="8">
         <f t="shared" si="0"/>
         <v>0.61458333333333315</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B31,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B31&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B31,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B31&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B31,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B31&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B31,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B31&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G31" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B31,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B31&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B31,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B31&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I31" s="8">
+      <c r="I31" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B31,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B31&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="5">
+    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="8">
         <f t="shared" si="0"/>
         <v>0.62499999999999978</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B32,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B32&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B32,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B32&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B32,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B32&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B32,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B32&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B32,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B32&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="8">
+      <c r="H32" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B32,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B32&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I32" s="8">
+      <c r="I32" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B32,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B32&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="5">
+    <row r="33" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="8">
         <f t="shared" si="0"/>
         <v>0.63541666666666641</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B33,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B33&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B33,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B33&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B33,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B33&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B33,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B33&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B33,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B33&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H33" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B33,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B33&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I33" s="8">
+      <c r="I33" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B33,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B33&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="5">
+    <row r="34" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="8">
         <f t="shared" si="0"/>
         <v>0.64583333333333304</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B34,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B34&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B34,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B34&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B34,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B34&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B34,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B34&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G34" s="8">
+      <c r="G34" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B34,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B34&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H34" s="8">
+      <c r="H34" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B34,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B34&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I34" s="8">
+      <c r="I34" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B34,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B34&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="5">
+    <row r="35" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="8">
         <f t="shared" si="0"/>
         <v>0.65624999999999967</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B35,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B35&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B35,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B35&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B35,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B35&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B35,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B35&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G35" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B35,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B35&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H35" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B35,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B35&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I35" s="8">
+      <c r="I35" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B35,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B35&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="5">
+    <row r="36" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="8">
         <f t="shared" si="0"/>
         <v>0.6666666666666663</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B36,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B36&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D36" s="8" t="str">
+      <c r="D36" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B36,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B36&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>SP-111</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B36,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B36&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F36" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B36,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B36&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B36,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B36&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H36" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B36,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B36&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I36" s="8">
+      <c r="I36" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B36,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B36&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="5">
+    <row r="37" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="8">
         <f t="shared" ref="B37:B56" si="1">B36+Increment</f>
         <v>0.67708333333333293</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B37,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B37&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="8" t="str">
+      <c r="D37" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B37,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B37&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>SP-111</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B37,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B37&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B37,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B37&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G37" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B37,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B37&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="8">
+      <c r="H37" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B37,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B37&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="8">
+      <c r="I37" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B37,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B37&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B38" s="5">
+    <row r="38" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="8">
         <f t="shared" si="1"/>
         <v>0.68749999999999956</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B38,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B38&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D38" s="8" t="str">
+      <c r="D38" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B38,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B38&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>SP-111</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B38,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B38&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F38" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B38,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B38&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B38,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B38&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H38" s="8">
+      <c r="H38" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B38,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B38&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I38" s="8">
+      <c r="I38" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B38,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B38&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B39" s="5">
+    <row r="39" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="8">
         <f t="shared" si="1"/>
         <v>0.69791666666666619</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B39,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B39&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D39" s="8" t="str">
+      <c r="D39" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B39,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B39&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>SP-111</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B39,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B39&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F39" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B39,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B39&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G39" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B39,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B39&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H39" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B39,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B39&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I39" s="8">
+      <c r="I39" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B39,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B39&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B40" s="5">
+    <row r="40" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="8">
         <f t="shared" si="1"/>
         <v>0.70833333333333282</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B40,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B40&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D40" s="8" t="str">
+      <c r="D40" s="9" t="str">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B40,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B40&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>SP-111</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E40" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B40,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B40&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F40" s="8">
+      <c r="F40" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B40,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B40&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G40" s="8">
+      <c r="G40" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B40,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B40&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H40" s="8">
+      <c r="H40" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B40,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B40&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I40" s="8">
+      <c r="I40" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B40,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B40&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B41" s="5">
+    <row r="41" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="8">
         <f t="shared" si="1"/>
         <v>0.71874999999999944</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B41,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B41&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D41" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B41,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B41&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E41" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B41,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B41&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F41" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B41,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B41&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G41" s="8">
+      <c r="G41" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B41,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B41&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H41" s="8">
+      <c r="H41" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B41,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B41&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I41" s="8">
+      <c r="I41" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B41,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B41&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B42" s="5">
+    <row r="42" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="8">
         <f t="shared" si="1"/>
         <v>0.72916666666666607</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B42,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B42&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D42" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B42,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B42&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E42" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B42,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B42&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F42" s="8">
+      <c r="F42" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B42,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B42&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G42" s="8">
+      <c r="G42" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B42,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B42&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="8">
+      <c r="H42" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B42,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B42&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I42" s="8">
+      <c r="I42" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B42,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B42&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B43" s="5">
+    <row r="43" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="8">
         <f t="shared" si="1"/>
         <v>0.7395833333333327</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C43" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B43,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B43&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D43" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B43,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B43&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E43" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B43,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B43&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F43" s="8">
+      <c r="F43" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B43,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B43&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="8">
+      <c r="G43" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B43,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B43&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H43" s="8">
+      <c r="H43" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B43,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B43&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I43" s="8">
+      <c r="I43" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B43,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B43&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B44" s="5">
+    <row r="44" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="8">
         <f t="shared" si="1"/>
         <v>0.74999999999999933</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C44" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B44,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B44&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D44" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B44,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B44&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E44" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B44,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B44&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F44" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B44,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B44&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G44" s="8">
+      <c r="G44" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B44,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B44&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H44" s="8">
+      <c r="H44" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B44,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B44&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I44" s="8">
+      <c r="I44" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B44,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B44&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B45" s="5">
+    <row r="45" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="8">
         <f t="shared" si="1"/>
         <v>0.76041666666666596</v>
       </c>
-      <c r="C45" s="8">
+      <c r="C45" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B45,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B45&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D45" s="8">
+      <c r="D45" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B45,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B45&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E45" s="8">
+      <c r="E45" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B45,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B45&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F45" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B45,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B45&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G45" s="8">
+      <c r="G45" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B45,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B45&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H45" s="8">
+      <c r="H45" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B45,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B45&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I45" s="8">
+      <c r="I45" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B45,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B45&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B46" s="5">
+    <row r="46" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="8">
         <f t="shared" si="1"/>
         <v>0.77083333333333259</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C46" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B46,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B46&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D46" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B46,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B46&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E46" s="8">
+      <c r="E46" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B46,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B46&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F46" s="8">
+      <c r="F46" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B46,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B46&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G46" s="8">
+      <c r="G46" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B46,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B46&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H46" s="8">
+      <c r="H46" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B46,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B46&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I46" s="8">
+      <c r="I46" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B46,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B46&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B47" s="5">
+    <row r="47" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="8">
         <f t="shared" si="1"/>
         <v>0.78124999999999922</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C47" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B47,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B47&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D47" s="8">
+      <c r="D47" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B47,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B47&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E47" s="8">
+      <c r="E47" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B47,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B47&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F47" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B47,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B47&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G47" s="8">
+      <c r="G47" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B47,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B47&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H47" s="8">
+      <c r="H47" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B47,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B47&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I47" s="8">
+      <c r="I47" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B47,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B47&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B48" s="5">
+    <row r="48" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="8">
         <f t="shared" si="1"/>
         <v>0.79166666666666585</v>
       </c>
-      <c r="C48" s="8">
+      <c r="C48" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B48,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B48&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D48" s="8">
+      <c r="D48" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B48,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B48&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E48" s="8">
+      <c r="E48" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B48,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B48&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F48" s="8">
+      <c r="F48" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B48,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B48&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G48" s="8">
+      <c r="G48" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B48,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B48&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H48" s="8">
+      <c r="H48" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B48,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B48&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I48" s="8">
+      <c r="I48" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B48,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B48&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B49" s="5">
+    <row r="49" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="8">
         <f t="shared" si="1"/>
         <v>0.80208333333333248</v>
       </c>
-      <c r="C49" s="8">
+      <c r="C49" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B49,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B49&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D49" s="8">
+      <c r="D49" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B49,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B49&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E49" s="8">
+      <c r="E49" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B49,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B49&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F49" s="8">
+      <c r="F49" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B49,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B49&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G49" s="8">
+      <c r="G49" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B49,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B49&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H49" s="8">
+      <c r="H49" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B49,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B49&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I49" s="8">
+      <c r="I49" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B49,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B49&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B50" s="5">
+    <row r="50" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="8">
         <f t="shared" si="1"/>
         <v>0.81249999999999911</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C50" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B50,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B50&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D50" s="8">
+      <c r="D50" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B50,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B50&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E50" s="8">
+      <c r="E50" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B50,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B50&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F50" s="8">
+      <c r="F50" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B50,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B50&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G50" s="8">
+      <c r="G50" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B50,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B50&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H50" s="8">
+      <c r="H50" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B50,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B50&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I50" s="8">
+      <c r="I50" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B50,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B50&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B51" s="5">
+    <row r="51" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="8">
         <f t="shared" si="1"/>
         <v>0.82291666666666574</v>
       </c>
-      <c r="C51" s="8">
+      <c r="C51" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B51,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B51&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D51" s="8">
+      <c r="D51" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B51,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B51&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E51" s="8">
+      <c r="E51" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B51,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B51&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F51" s="8">
+      <c r="F51" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B51,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B51&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G51" s="8">
+      <c r="G51" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B51,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B51&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H51" s="8">
+      <c r="H51" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B51,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B51&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I51" s="8">
+      <c r="I51" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B51,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B51&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B52" s="5">
+    <row r="52" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="8">
         <f t="shared" si="1"/>
         <v>0.83333333333333237</v>
       </c>
-      <c r="C52" s="8">
+      <c r="C52" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B52,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B52&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D52" s="8">
+      <c r="D52" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B52,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B52&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E52" s="8">
+      <c r="E52" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B52,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B52&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F52" s="8">
+      <c r="F52" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B52,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B52&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G52" s="8">
+      <c r="G52" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B52,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B52&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H52" s="8">
+      <c r="H52" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B52,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B52&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I52" s="8">
+      <c r="I52" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B52,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B52&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B53" s="5">
+    <row r="53" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="8">
         <f t="shared" si="1"/>
         <v>0.843749999999999</v>
       </c>
-      <c r="C53" s="8">
+      <c r="C53" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B53,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B53&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D53" s="8">
+      <c r="D53" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B53,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B53&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E53" s="8">
+      <c r="E53" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B53,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B53&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F53" s="8">
+      <c r="F53" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B53,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B53&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G53" s="8">
+      <c r="G53" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B53,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B53&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H53" s="8">
+      <c r="H53" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B53,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B53&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I53" s="8">
+      <c r="I53" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B53,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B53&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B54" s="5">
+    <row r="54" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="8">
         <f t="shared" si="1"/>
         <v>0.85416666666666563</v>
       </c>
-      <c r="C54" s="8">
+      <c r="C54" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B54,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B54&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D54" s="8">
+      <c r="D54" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B54,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B54&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E54" s="8">
+      <c r="E54" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B54,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B54&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F54" s="8">
+      <c r="F54" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B54,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B54&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G54" s="8">
+      <c r="G54" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B54,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B54&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H54" s="8">
+      <c r="H54" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B54,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B54&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I54" s="8">
+      <c r="I54" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B54,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B54&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B55" s="5">
+    <row r="55" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="8">
         <f t="shared" si="1"/>
         <v>0.86458333333333226</v>
       </c>
-      <c r="C55" s="8">
+      <c r="C55" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B55,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B55&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D55" s="8">
+      <c r="D55" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B55,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B55&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E55" s="8">
+      <c r="E55" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B55,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B55&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F55" s="8">
+      <c r="F55" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B55,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B55&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G55" s="8">
+      <c r="G55" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B55,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B55&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H55" s="8">
+      <c r="H55" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B55,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B55&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I55" s="8">
+      <c r="I55" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B55,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B55&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B56" s="5">
+    <row r="56" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="8">
         <f t="shared" si="1"/>
         <v>0.87499999999999889</v>
       </c>
-      <c r="C56" s="8">
+      <c r="C56" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SUNDAY]])*(ROUNDDOWN($B56,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B56&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="D56" s="8">
+      <c r="D56" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[MONDAY]])*(ROUNDDOWN($B56,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B56&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="E56" s="8">
+      <c r="E56" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[TUESDAY]])*(ROUNDDOWN($B56,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B56&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F56" s="8">
+      <c r="F56" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[WEDNESDAY]])*(ROUNDDOWN($B56,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B56&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="G56" s="8">
+      <c r="G56" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[THURSDAY]])*(ROUNDDOWN($B56,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B56&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="H56" s="8">
+      <c r="H56" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[FRIDAY]])*(ROUNDDOWN($B56,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B56&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="I56" s="8">
+      <c r="I56" s="9">
         <f>IFERROR(INDEX(ClassList[],MATCH(SUMPRODUCT((ClassList[DAY]=ClassSchedule[[#Headers],[SATURDAY]])*(ROUNDDOWN($B56,10)&gt;=ROUNDDOWN(ClassList[START TIME],10))*($B56&lt;=ClassList[END TIME]),ClassList[UNIQUE]),ClassList[UNIQUE],0),2),0)</f>
         <v>0</v>
       </c>
@@ -3292,71 +3338,71 @@
     <mergeCell ref="I1:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:I56">
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="29" priority="2">
       <formula>(C4=C3)*(C$3=ThisWeekday)*(C4&lt;&gt;0)*($B4&lt;Cal_Endtime)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="3">
+    <cfRule type="expression" dxfId="28" priority="3">
       <formula>(C$3=ThisWeekday)*(C4&lt;&gt;0)*($B4&lt;Cal_Endtime)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="27" priority="6">
       <formula>(C4=C3)*(C4&lt;&gt;0)*($B4&lt;Cal_Endtime)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="8">
+    <cfRule type="expression" dxfId="26" priority="8">
       <formula>(C4&lt;&gt;0)*($B4&lt;Cal_Endtime)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>(C$3=ThisWeekday)*($B4&lt;Cal_Endtime)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="298">
+    <cfRule type="expression" dxfId="24" priority="298">
       <formula>C4=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:I3">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>(B3=ThisWeekday)*($B4&lt;Cal_Endtime)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:I56">
-    <cfRule type="expression" dxfId="11" priority="400">
+    <cfRule type="expression" dxfId="22" priority="400">
       <formula>($B4&lt;=CurrentTime)*($B5&gt;=CurrentTime)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="401">
+    <cfRule type="expression" dxfId="21" priority="401">
       <formula>(ROW(B4)&lt;ROW(INDEX($B$4:$B81,MATCH(Cal_Endtime,$B$4:$B$81,1),1))+1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="402">
+    <cfRule type="expression" dxfId="20" priority="402">
       <formula>B4=B3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="403" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="403" stopIfTrue="1">
       <formula>(B4&gt;Cal_Endtime)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="404">
+    <cfRule type="expression" dxfId="18" priority="404">
       <formula>INDEX($B$4:$B81,MATCH(Cal_Endtime,$B$4:$B$81,1),1)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a start time from the list. Select CANCEL, and then press ALT+DOWN ARROW to select start time from the drop-down list" prompt="Enter schedule start time in this cell. Press ALT+DOWN ARROW to open the drop-down list, and then press ENTER to select the time" sqref="G2">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a start time from the list. Select CANCEL, and then press ALT+DOWN ARROW to select start time from the drop-down list" prompt="Enter schedule start time in this cell. Press ALT+DOWN ARROW to open the drop-down list, and then press ENTER to select the time" sqref="G2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"8:00 AM,9:00 AM,10:00 AM,11:00 AM,12:00 PM,1:00 PM,2:00 PM,3:00 PM,4:00 PM,5:00 PM"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a time interval from the list. Select CANCEL, and then press ALT+DOWN ARROW to select time interval from the drop-down list" prompt="Enter time interval in this cell. Press ALT+DOWN ARROW to open the drop-down list, and then press ENTER to select time interval" sqref="H2">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a time interval from the list. Select CANCEL, and then press ALT+DOWN ARROW to select time interval from the drop-down list" prompt="Enter time interval in this cell. Press ALT+DOWN ARROW to open the drop-down list, and then press ENTER to select time interval" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"15 MIN,20 MIN,30 MIN,40 MIN,45 MIN,60 MIN"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="To update Class Schedule, modify Schedule Start in cell G2 &amp; Time Interval in cell H2. Add class information in Class List worksheet. Cell I1 navigates to Class List worksheet" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class Schedule Table, below, is automatically updated from entries in the Class List table in the Class List worksheet. Add rows to the end of the table to extend the schedule" sqref="B1:F2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter schedule start time in cell G2" sqref="G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter time interval in cell H2" sqref="H1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Sunday is automatically updated using entries from Class List worksheet" sqref="C3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Monday is automatically updated using entries from Class List worksheet" sqref="D3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Tuesday is automatically updated using entries from Class List worksheet" sqref="E3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Wednesday is automatically updated using entries from Class List worksheet" sqref="F3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Thursday is automatically updated using entries from Class List worksheet" sqref="G3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Friday is automatically updated using entries from Class List worksheet" sqref="H3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Saturday is automatically updated using entries from Class List worksheet" sqref="I3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This column is generated based on Start Time in cell G2 and Time Interval in cell H2" sqref="B3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Schedule start time determined by the time entered in cell G2" sqref="B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to Class List worksheet" sqref="I1:I2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="To update Class Schedule, modify Schedule Start in cell G2 &amp; Time Interval in cell H2. Add class information in Class List worksheet. Cell I1 navigates to Class List worksheet" sqref="A1" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class Schedule Table, below, is automatically updated from entries in the Class List table in the Class List worksheet. Add rows to the end of the table to extend the schedule" sqref="B1:F2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter schedule start time in cell G2" sqref="G1" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter time interval in cell H2" sqref="H1" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Sunday is automatically updated using entries from Class List worksheet" sqref="C3" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Monday is automatically updated using entries from Class List worksheet" sqref="D3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Tuesday is automatically updated using entries from Class List worksheet" sqref="E3" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Wednesday is automatically updated using entries from Class List worksheet" sqref="F3" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Thursday is automatically updated using entries from Class List worksheet" sqref="G3" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Friday is automatically updated using entries from Class List worksheet" sqref="H3" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Class schedule for Saturday is automatically updated using entries from Class List worksheet" sqref="I3" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This column is generated based on Start Time in cell G2 and Time Interval in cell H2" sqref="B3" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Schedule start time determined by the time entered in cell G2" sqref="B4" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to Class List worksheet" sqref="I1:I2" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I1" location="'Class List'!A1" tooltip="Select to navigate to Class List worksheet" display="Class List"/>
+    <hyperlink ref="I1" location="'Class List'!A1" tooltip="Select to navigate to Class List worksheet" display="Class List" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3375,82 +3421,82 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2">
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:H25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="1" customWidth="1"/>
-    <col min="5" max="7" width="22.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="10" customWidth="1"/>
+    <col min="5" max="7" width="22.125" style="10" customWidth="1"/>
     <col min="8" max="8" width="10.5" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="2.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="2.625" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="16" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="16"/>
-    </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="4" t="s">
+      <c r="H1" s="17"/>
+    </row>
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="11" t="s">
         <v>26</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8" t="s">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="8">
         <v>0.54166666666666596</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="8">
         <v>0.58333333333333337</v>
       </c>
       <c r="H3" s="2">
@@ -3458,23 +3504,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="8" t="s">
+    <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="8">
         <v>0.54166666666666596</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="8">
         <v>0.58333333333333337</v>
       </c>
       <c r="H4" s="2">
@@ -3482,23 +3528,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="8">
         <v>0.66666666666666663</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="8">
         <v>0.70833333333333337</v>
       </c>
       <c r="H5" s="2">
@@ -3506,23 +3552,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="8">
         <v>0.45833333333333331</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="8">
         <v>0.5</v>
       </c>
       <c r="H6" s="2">
@@ -3530,23 +3576,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="8" t="s">
+    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="8">
         <v>0.45833333333333287</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="8">
         <v>0.5</v>
       </c>
       <c r="H7" s="2">
@@ -3554,23 +3600,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="8" t="s">
+    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="8">
         <v>0.34027777777777773</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="8">
         <v>0.38541666666666669</v>
       </c>
       <c r="H8" s="2">
@@ -3578,23 +3624,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="8" t="s">
+    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="8">
         <v>0.34027777777777773</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="8">
         <v>0.38541666666666669</v>
       </c>
       <c r="H9" s="3">
@@ -3602,23 +3648,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="8" t="s">
+    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="8">
         <v>0.34027777777777773</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="8">
         <v>0.38541666666666669</v>
       </c>
       <c r="H10" s="3">
@@ -3626,211 +3672,211 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="11" t="s">
+    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="11" t="s">
+    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="13" t="s">
+    <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="11" t="s">
+    <row r="14" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
       <c r="H14" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="13" t="s">
+    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
       <c r="H15" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="13" t="s">
+    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
       <c r="H16" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="13" t="s">
+    <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
       <c r="H17" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="13" t="s">
+    <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
       <c r="H18" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="13" t="s">
+    <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
       <c r="H19" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="13" t="s">
+    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
       <c r="H20" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="13" t="s">
+    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
       <c r="H21" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="13" t="s">
+    <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
       <c r="H22" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="13" t="s">
+    <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
       <c r="H23" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="13" t="s">
+    <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
       <c r="H24" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="13" t="s">
+    <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
       <c r="H25" s="3">
         <f>ROW()-ROW(ClassList[[#Headers],[UNIQUE]])</f>
         <v>23</v>
@@ -3842,21 +3888,21 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <dataValidations count="10">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to Class Schedule worksheet" sqref="G1:H1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Class in this column" sqref="B2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class ID in this column" sqref="C2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class Day in this column.  In each cell of this column, Press ALT+DOWN ARROW to open the drop-down list, and then press ENTER to select the Day" sqref="D2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class Location in this column" sqref="E2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class Start Time in this column" sqref="F2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class End Time in this column" sqref="G2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a class list to update Class Schedule by updating the Class List table. Use table filters to get specific class or date. Cell G1 navigates to Class Schedule" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This list is used to create the Class Schedule on the Class Schedule worksheet. Update the Class List table, below, to automatically update Class Schedule" sqref="B1:F1"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a day from the list. Select CANCEL, and then press ALT+DOWN ARROW to select from the drop-down list" sqref="D3:D25">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to Class Schedule worksheet" sqref="G1:H1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Class in this column" sqref="B2" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class ID in this column" sqref="C2" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class Day in this column.  In each cell of this column, Press ALT+DOWN ARROW to open the drop-down list, and then press ENTER to select the Day" sqref="D2" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class Location in this column" sqref="E2" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class Start Time in this column" sqref="F2" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter class End Time in this column" sqref="G2" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a class list to update Class Schedule by updating the Class List table. Use table filters to get specific class or date. Cell G1 navigates to Class Schedule" sqref="A1" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This list is used to create the Class Schedule on the Class Schedule worksheet. Update the Class List table, below, to automatically update Class Schedule" sqref="B1:F1" xr:uid="{00000000-0002-0000-0100-000008000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a day from the list. Select CANCEL, and then press ALT+DOWN ARROW to select from the drop-down list" sqref="D3:D25" xr:uid="{00000000-0002-0000-0100-000009000000}">
       <formula1>"SUNDAY,MONDAY,TUESDAY,WEDNESDAY,THURSDAY,FRIDAY,SATURDAY"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G1:H1" location="'Class Schedule'!A1" tooltip="Select to navigate to Class Schedule worksheet" display="Class Schedule"/>
+    <hyperlink ref="G1:H1" location="'Class Schedule'!A1" tooltip="Select to navigate to Class Schedule worksheet" display="Class Schedule" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>